<commit_message>
continunando teste - arquivo certo
</commit_message>
<xml_diff>
--- a/Apple.xlsx
+++ b/Apple.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusta\OneDrive\Área de Trabalho\Insper\2º SEMESTRE\CIÊNCIA DOS DADOS\Projeto 1\Arquivos bb\projeto1data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="352" documentId="11_57AEF00966831FE8EC869A7057F8FC45E12FF8D4" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{51DE564B-6FF6-410F-9319-01F9A5737020}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04444B85-04CE-4B7A-AFA8-118A02817C7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -2578,8 +2578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="G135" sqref="G135"/>
+    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3964,103 +3964,130 @@
       <c r="A172" t="s">
         <v>171</v>
       </c>
+      <c r="B172">
+        <v>1</v>
+      </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>172</v>
       </c>
+      <c r="B173">
+        <v>0</v>
+      </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>173</v>
       </c>
+      <c r="B174">
+        <v>1</v>
+      </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>174</v>
       </c>
+      <c r="B175">
+        <v>0</v>
+      </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>191</v>
       </c>
@@ -4620,8 +4647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F323"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="E139" sqref="E139"/>
+    <sheetView topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="B202" sqref="B202:B207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5834,293 +5861,449 @@
       <c r="A150" t="s">
         <v>450</v>
       </c>
+      <c r="B150">
+        <v>1</v>
+      </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>451</v>
       </c>
+      <c r="B151">
+        <v>1</v>
+      </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>452</v>
       </c>
+      <c r="B152">
+        <v>0</v>
+      </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>453</v>
       </c>
+      <c r="B153">
+        <v>1</v>
+      </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>454</v>
       </c>
+      <c r="B154">
+        <v>0</v>
+      </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>455</v>
       </c>
+      <c r="B155">
+        <v>1</v>
+      </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>456</v>
       </c>
+      <c r="B156">
+        <v>0</v>
+      </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>457</v>
       </c>
+      <c r="B157">
+        <v>1</v>
+      </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>458</v>
       </c>
+      <c r="B158">
+        <v>1</v>
+      </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>459</v>
       </c>
+      <c r="B159">
+        <v>1</v>
+      </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>508</v>
       </c>

</xml_diff>

<commit_message>
terminando teste e treinamento
</commit_message>
<xml_diff>
--- a/Apple.xlsx
+++ b/Apple.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiago\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04444B85-04CE-4B7A-AFA8-118A02817C7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4ED673-29C1-4010-B8BA-335AED574C9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2578,8 +2578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="B181" sqref="B181"/>
+    <sheetView tabSelected="1" topLeftCell="A203" workbookViewId="0">
+      <selection activeCell="E219" sqref="E219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4036,605 +4036,976 @@
       <c r="A181" t="s">
         <v>180</v>
       </c>
+      <c r="B181">
+        <v>1</v>
+      </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>181</v>
       </c>
+      <c r="B182">
+        <v>1</v>
+      </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>182</v>
       </c>
+      <c r="B183">
+        <v>1</v>
+      </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>183</v>
       </c>
+      <c r="B184">
+        <v>0</v>
+      </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>184</v>
       </c>
+      <c r="B185">
+        <v>0</v>
+      </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>185</v>
       </c>
+      <c r="B186">
+        <v>1</v>
+      </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>186</v>
       </c>
+      <c r="B187">
+        <v>0</v>
+      </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>187</v>
       </c>
+      <c r="B188">
+        <v>0</v>
+      </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>188</v>
       </c>
+      <c r="B189">
+        <v>1</v>
+      </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>189</v>
       </c>
+      <c r="B190">
+        <v>0</v>
+      </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>190</v>
       </c>
+      <c r="B191">
+        <v>1</v>
+      </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B219">
+        <v>1</v>
+      </c>
+      <c r="D219">
+        <f>COUNTIF(B2:B301,1)</f>
+        <v>165</v>
+      </c>
+      <c r="E219">
+        <f>COUNTIF(B2:B301,0)</f>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B238">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B254">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B255">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A256" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B258">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B262">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B267">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B268">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B269">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B270">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B271">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B272">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B273">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B274">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B277">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B278">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B279">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B280">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B281">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B283">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B285">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B286">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B287">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B288">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B289">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B290">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B291">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B292">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B293">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B294">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B295">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B296">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B297">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B298">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="B300">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>300</v>
+      </c>
+      <c r="B301">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4647,8 +5018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F323"/>
   <sheetViews>
-    <sheetView topLeftCell="A192" workbookViewId="0">
-      <selection activeCell="B202" sqref="B202:B207"/>
+    <sheetView topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="F140" sqref="F140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5769,12 +6140,12 @@
         <v>0</v>
       </c>
       <c r="E139">
-        <f>COUNTIF(B1:B149,1)</f>
-        <v>74</v>
+        <f>COUNTIF(B2:B201,1)</f>
+        <v>104</v>
       </c>
       <c r="F139">
-        <f>COUNTIF(B1:B149,0)</f>
-        <v>74</v>
+        <f>COUNTIF(B2:B201,0)</f>
+        <v>96</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>